<commit_message>
fix -> ajuste de cadastro_empresas
</commit_message>
<xml_diff>
--- a/static/assets/arquivos/empregados.xlsx
+++ b/static/assets/arquivos/empregados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Nome</t>
   </si>
@@ -28,7 +28,19 @@
     <t>Guilherme</t>
   </si>
   <si>
+    <t>Paulo</t>
+  </si>
+  <si>
+    <t>Git e Github</t>
+  </si>
+  <si>
     <t>celente.guilherme@outlook.com</t>
+  </si>
+  <si>
+    <t>progeri@yahoo.com</t>
+  </si>
+  <si>
+    <t>guilherme.celente@escola.pr.gov.br</t>
   </si>
   <si>
     <t>rtRfd34</t>
@@ -389,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -411,10 +423,32 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>